<commit_message>
scrape and prep all empirical estimate data
</commit_message>
<xml_diff>
--- a/Empirical estimates of confounding bias/Raw data/Golder data/Golder forest plot scraped.xlsx
+++ b/Empirical estimates of confounding bias/Raw data/Golder data/Golder forest plot scraped.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmathur/Dropbox/Personal computer/Independent studies/2021/AR-T (Ann Rev tutorial)/Git (AR-T)/Empirical estimates of confounding bias/Raw data/Golder data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63275B17-72E1-5241-BBDB-500598106140}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF908F56-95B5-C544-AB8E-1676216F7D2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="1200" windowWidth="33600" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4180" yWindow="5780" windowWidth="33600" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <r>
       <rPr>
@@ -89,16 +89,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">1.19 [1.00. 1.41] </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve">0.90 [0.72, 1.12] </t>
     </r>
   </si>
@@ -169,16 +159,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">1.12 [0.91. 1.38] </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve">0.85 [0.59, 1.21] </t>
     </r>
   </si>
@@ -189,16 +169,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">0.37 [0.13. 1.04] </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve">0.37 [0.13, 1.00] </t>
     </r>
   </si>
@@ -219,16 +189,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">0.41 [0.15. 1.11] </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve">0.26 [0.06, 1.23] </t>
     </r>
   </si>
@@ -239,16 +199,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">0.52 [0.06. 4.83] </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve">0.78 [0.35, 1.72] </t>
     </r>
   </si>
@@ -289,16 +239,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">1.40 [0.61. 3.24] </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve">1.62 [1.07, 2.44] </t>
     </r>
   </si>
@@ -309,16 +249,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">0.87 [0.45. 1.68] </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve">1.10 [0.15, 8.17] </t>
     </r>
   </si>
@@ -389,16 +319,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">1.21 [0.81. 1.81] </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve">1.99 [0.64, 6.18) </t>
     </r>
   </si>
@@ -449,16 +369,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">0.32 [0.20. 0.52] </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve">1.45 [0.74, 2.82] </t>
     </r>
   </si>
@@ -489,16 +399,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">0.09 [0.02. 0.48) </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve">0.97 [0.72, 1.30] </t>
     </r>
   </si>
@@ -519,16 +419,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">1.31 [0.86. 1.99] </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve">0.78 [0.36, 1.72] </t>
     </r>
   </si>
@@ -599,18 +489,47 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">0.42 [0.19. 0.92] </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>1.09 [0.35, 3.44]</t>
     </r>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.19 [1.00, 1.41] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.37 [0.13, 1.04] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.41 [0.15, 1.11] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.52 [0.06, 4.83] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.40 [0.61, 3.24] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.87 [0.45, 1.68] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.21 [0.81, 1.81] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.32 [0.20, 0.52] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.09 [0.02, 0.48) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.31 [0.86, 1.99] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.42 [0.19, 0.92] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.12 [0.91, 1.38] </t>
   </si>
 </sst>
 </file>
@@ -976,300 +895,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A58"/>
+  <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="9" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="10" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="11" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="12" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="13" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="14" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="15" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="19" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+    <row r="20" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="22" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="24" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    <row r="25" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="26" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="27" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="29" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="31" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="32" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="34" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="36" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+    <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+    <row r="39" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="40" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="41" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="42" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="43" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="45" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="46" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+    <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+    <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>